<commit_message>
Estilo linha do tempo
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="COMUNICACAO" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -998,7 +998,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,6 +1011,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1036,8 +1046,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1049,8 +1060,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Separador de milhares 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1583,10 +1595,10 @@
   <dimension ref="A1:FA19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="DP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" sqref="A1:FA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Hiperlinks - nova branch mapa
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -4008,9 +4008,6 @@
           </cell>
         </row>
         <row r="15">
-          <cell r="A15">
-            <v>8</v>
-          </cell>
           <cell r="B15" t="str">
             <v>PIU Pacaembu</v>
           </cell>
@@ -7943,8 +7940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EX20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BG10" sqref="BG10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12898,8 +12895,7 @@
       </c>
     </row>
     <row r="9" spans="1:154">
-      <c r="A9" t="str">
-        <f>CLEAN(IF([1]BD!A$6="P",[1]BD!A15,""))</f>
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="str">
@@ -18322,7 +18318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:154" ht="48">
+    <row r="19" spans="1:154" ht="36">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -18626,7 +18622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:154" ht="48">
+    <row r="20" spans="1:154" ht="36">
       <c r="A20" s="2">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Preenchimento em multiply mapa / legenda mapa
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -481,7 +481,343 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Separador de milhares" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="140">
+  <dxfs count="168">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -9742,6 +10078,7 @@
       <sheetName val="De-Para classificatório"/>
       <sheetName val="Personal"/>
       <sheetName val="História"/>
+      <sheetName val="PIU_Monitoramento"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -10621,6 +10958,9 @@
           <cell r="BE8" t="str">
             <v>-</v>
           </cell>
+          <cell r="BF8" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BG8" t="str">
             <v>-</v>
           </cell>
@@ -10649,6 +10989,12 @@
             <v>-</v>
           </cell>
           <cell r="BP8" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BQ8" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR8" t="str">
             <v>-</v>
           </cell>
           <cell r="BS8" t="str">
@@ -13691,9 +14037,6 @@
           </cell>
           <cell r="EW14" t="str">
             <v>-</v>
-          </cell>
-          <cell r="EX14">
-            <v>2</v>
           </cell>
         </row>
         <row r="15">
@@ -14333,6 +14676,9 @@
           <cell r="BD16" t="str">
             <v>-</v>
           </cell>
+          <cell r="BE16" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BF16" t="str">
             <v>-</v>
           </cell>
@@ -14364,6 +14710,12 @@
             <v>-</v>
           </cell>
           <cell r="BP16" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BQ16" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR16" t="str">
             <v>-</v>
           </cell>
           <cell r="BS16" t="str">
@@ -14617,7 +14969,7 @@
             <v>-</v>
           </cell>
           <cell r="EX16">
-            <v>3</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="17">
@@ -14826,6 +15178,12 @@
           <cell r="BP17" t="str">
             <v>-</v>
           </cell>
+          <cell r="BQ17" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR17" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BS17" t="str">
             <v>-</v>
           </cell>
@@ -15278,6 +15636,12 @@
           <cell r="BP18" t="str">
             <v>-</v>
           </cell>
+          <cell r="BQ18" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR18" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BS18" t="str">
             <v>-</v>
           </cell>
@@ -15734,6 +16098,12 @@
           <cell r="BP19" t="str">
             <v>-</v>
           </cell>
+          <cell r="BQ19" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR19" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BS19" t="str">
             <v>-</v>
           </cell>
@@ -16039,6 +16409,9 @@
           <cell r="Q20" t="str">
             <v>-</v>
           </cell>
+          <cell r="R20" t="str">
+            <v>-</v>
+          </cell>
           <cell r="S20" t="str">
             <v>-</v>
           </cell>
@@ -16187,6 +16560,12 @@
             <v>-</v>
           </cell>
           <cell r="BP20" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BQ20" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR20" t="str">
             <v>-</v>
           </cell>
           <cell r="BS20" t="str">
@@ -16647,6 +17026,12 @@
           <cell r="BP21" t="str">
             <v>-</v>
           </cell>
+          <cell r="BQ21" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR21" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BS21" t="str">
             <v>-</v>
           </cell>
@@ -17102,6 +17487,12 @@
           <cell r="BP22" t="str">
             <v>-</v>
           </cell>
+          <cell r="BQ22" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="BR22" t="str">
+            <v>-</v>
+          </cell>
           <cell r="BS22" t="str">
             <v>-</v>
           </cell>
@@ -17716,6 +18107,27 @@
           <cell r="DQ23" t="str">
             <v>PL 723/2015</v>
           </cell>
+          <cell r="DR23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DS23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DT23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DU23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DV23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DW23" t="str">
+            <v>-</v>
+          </cell>
+          <cell r="DX23" t="str">
+            <v>-</v>
+          </cell>
           <cell r="DY23" t="str">
             <v>PDE</v>
           </cell>
@@ -17732,6 +18144,9 @@
           </cell>
           <cell r="EM23" t="str">
             <v>Lei</v>
+          </cell>
+          <cell r="EX23">
+            <v>7</v>
           </cell>
         </row>
         <row r="24">
@@ -19127,10 +19542,17 @@
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="6">
+        <row r="3">
+          <cell r="D3" t="str">
+            <v>Status</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
+      <sheetData sheetId="10" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -30443,142 +30865,142 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="139" priority="28" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="167" priority="28" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="138" priority="27" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="166" priority="27" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="137" priority="26" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="165" priority="26" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="136" priority="25" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="164" priority="25" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="135" priority="24" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="163" priority="24" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="134" priority="23" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="162" priority="23" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="133" priority="22" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="161" priority="22" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="132" priority="21" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="160" priority="21" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="131" priority="20" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="159" priority="20" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="130" priority="19" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="158" priority="19" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="129" priority="18" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="157" priority="18" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="128" priority="17" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="156" priority="17" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="127" priority="16" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="155" priority="16" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="126" priority="15" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="154" priority="15" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="125" priority="14" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="153" priority="14" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="124" priority="13" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="152" priority="13" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="123" priority="12" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="151" priority="12" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="122" priority="11" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="150" priority="11" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="121" priority="10" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="149" priority="10" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="120" priority="9" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="148" priority="9" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="119" priority="8" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="147" priority="8" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="118" priority="7" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="146" priority="7" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="117" priority="6" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="145" priority="6" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="116" priority="5" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="144" priority="5" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="115" priority="4" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="143" priority="4" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="114" priority="3" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="142" priority="3" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="113" priority="2" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="141" priority="2" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="112" priority="1" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="140" priority="1" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30606,10 +31028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:EX34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4605" topLeftCell="EA1" activePane="topRight"/>
-      <selection activeCell="A14" sqref="A14:XFD14"/>
-      <selection pane="topRight" activeCell="EX14" sqref="EX14"/>
+    <sheetView tabSelected="1" topLeftCell="DY1" workbookViewId="0">
+      <selection activeCell="EX8" sqref="EX8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -31469,7 +31889,7 @@
       </c>
       <c r="BF2" t="str">
         <f>CLEAN(IF([2]BD!BF$6="P",[2]BD!BF8,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BG2" t="str">
         <f>CLEAN(IF([2]BD!BG$6="P",[2]BD!BG8,""))</f>
@@ -31513,11 +31933,11 @@
       </c>
       <c r="BQ2" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ8,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR2" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR8,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS2" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS8,""))</f>
@@ -35559,8 +35979,7 @@
         <f>CLEAN(IF([2]BD!EW$6="P",[2]BD!EW14,""))</f>
         <v/>
       </c>
-      <c r="EX8" t="str">
-        <f>CLEAN(IF([2]BD!EX$6="P",[2]BD!EX14,""))</f>
+      <c r="EX8">
         <v>2</v>
       </c>
     </row>
@@ -36409,7 +36828,7 @@
       </c>
       <c r="BE10" t="str">
         <f>CLEAN(IF([2]BD!BE$6="P",[2]BD!BE16,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BF10" t="str">
         <f>CLEAN(IF([2]BD!BF$6="P",[2]BD!BF16,""))</f>
@@ -36457,11 +36876,11 @@
       </c>
       <c r="BQ10" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ16,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR10" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR16,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS10" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS16,""))</f>
@@ -36797,7 +37216,7 @@
       </c>
       <c r="EX10" t="str">
         <f>CLEAN(IF([2]BD!EX$6="P",[2]BD!EX16,""))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:154">
@@ -37075,11 +37494,11 @@
       </c>
       <c r="BQ11" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ17,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR11" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR17,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS11" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS17,""))</f>
@@ -37693,11 +38112,11 @@
       </c>
       <c r="BQ12" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ18,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR12" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR18,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS12" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS18,""))</f>
@@ -38311,11 +38730,11 @@
       </c>
       <c r="BQ13" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ22,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR13" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR22,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS13" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS22,""))</f>
@@ -39141,31 +39560,31 @@
       </c>
       <c r="DR14" t="str">
         <f>CLEAN(IF([2]BD!DR$6="P",[2]BD!DR23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DS14" t="str">
         <f>CLEAN(IF([2]BD!DS$6="P",[2]BD!DS23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DT14" t="str">
         <f>CLEAN(IF([2]BD!DT$6="P",[2]BD!DT23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DU14" s="2" t="str">
         <f>CLEAN(IF([2]BD!DU$6="P",[2]BD!DU23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DV14" t="str">
         <f>CLEAN(IF([2]BD!DV$6="P",[2]BD!DV23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DW14" t="str">
         <f>CLEAN(IF([2]BD!DW$6="P",[2]BD!DW23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DX14" t="str">
         <f>CLEAN(IF([2]BD!DX$6="P",[2]BD!DX23,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="DY14" t="str">
         <f>CLEAN(IF([2]BD!DY$6="P",[2]BD!DY23,""))</f>
@@ -39267,7 +39686,8 @@
         <f>CLEAN(IF([2]BD!EW$6="P",[2]BD!EW23,""))</f>
         <v/>
       </c>
-      <c r="EX14">
+      <c r="EX14" t="str">
+        <f>CLEAN(IF([2]BD!EX$6="P",[2]BD!EX23,""))</f>
         <v>7</v>
       </c>
     </row>
@@ -40782,11 +41202,11 @@
       </c>
       <c r="BQ17" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ19,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR17" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR19,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS17" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS19,""))</f>
@@ -41400,11 +41820,11 @@
       </c>
       <c r="BQ18" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ20,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR18" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR20,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS18" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS20,""))</f>
@@ -42018,11 +42438,11 @@
       </c>
       <c r="BQ19" t="str">
         <f>CLEAN(IF([2]BD!BQ$6="P",[2]BD!BQ21,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BR19" t="str">
         <f>CLEAN(IF([2]BD!BR$6="P",[2]BD!BR21,""))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="BS19" t="str">
         <f>CLEAN(IF([2]BD!BS$6="P",[2]BD!BS21,""))</f>
@@ -42994,6 +43414,146 @@
     <row r="33" ht="18" customHeight="1"/>
     <row r="34" ht="18" customHeight="1"/>
   </sheetData>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="138" priority="139" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="137" priority="138" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="136" priority="137" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="135" priority="136" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="134" priority="135" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="132" priority="133" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="131" priority="132" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="129" priority="130" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="128" priority="129" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="126" priority="127" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="125" priority="126" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="123" priority="124" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="122" priority="123" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="120" priority="121" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="119" priority="120" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="117" priority="118" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="116" priority="117" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="114" priority="115" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="113" priority="114" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
     <cfRule type="containsText" dxfId="111" priority="112" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
@@ -43064,12 +43624,12 @@
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 C17:C18 B17">
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
     <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 C17:C18 B17">
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
     <cfRule type="containsText" dxfId="96" priority="97" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
@@ -43094,24 +43654,24 @@
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C20">
+  <conditionalFormatting sqref="B18:C20">
     <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="PIU">
-      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:C20">
+  <conditionalFormatting sqref="B18:C20">
     <cfRule type="containsText" dxfId="90" priority="91" operator="containsText" text="Projeto">
-      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 C18">
+  <conditionalFormatting sqref="B18:B20 C18 C20">
     <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="PIU">
-      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20 C18">
+  <conditionalFormatting sqref="B18:B20 C18 C20">
     <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Projeto">
-      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">

</xml_diff>

<commit_message>
Finaliza primeira versao para publicar
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="26835" windowHeight="12090"/>
+    <workbookView xWindow="-300" yWindow="15" windowWidth="23790" windowHeight="10020"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,679 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="84">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -411,247 +1083,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>41415</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>33131</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>364436</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>207066</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!Menu_inicial" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo de cantos arredondados 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="41415" y="33131"/>
-          <a:ext cx="627821" cy="154885"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx2">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="88900" h="88900"/>
-          <a:bevelB w="88900" h="88900"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" b="1"/>
-            <a:t>Menu</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" b="1" baseline="0"/>
-            <a:t> inicial</a:t>
-          </a:r>
-          <a:endParaRPr lang="pt-BR" sz="1400" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>430696</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>16564</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1308653</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>198783</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!SalvarBaseExterno" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Retângulo de cantos arredondados 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="668821" y="16564"/>
-          <a:ext cx="1657" cy="172694"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="F4750C"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="88900" h="88900"/>
-          <a:bevelB w="88900" h="88900"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1"/>
-            <a:t>Exportar xls</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>430695</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>256760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1283804</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>455543</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!writeToCSVfile" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Retângulo de cantos arredondados 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="668820" y="190085"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="F4750C"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="88900" h="88900"/>
-          <a:bevelB w="88900" h="88900"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="b"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" b="1"/>
-            <a:t>Exportar csv</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="COMUNICACAO"/>
       <sheetName val="BD"/>
       <sheetName val="Menu inicial"/>
       <sheetName val="Ficha individual"/>
@@ -662,8 +1098,14 @@
       <sheetName val="Personal"/>
       <sheetName val="História"/>
     </sheetNames>
+    <definedNames>
+      <definedName name="Menu_inicial"/>
+      <definedName name="SalvarBaseExterno"/>
+      <definedName name="writeToCSVfile"/>
+    </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="1">
           <cell r="A1" t="str">
             <v>ID_rev</v>
@@ -1861,7 +2303,7 @@
             <v>SEP</v>
           </cell>
           <cell r="J9" t="str">
-            <v>Consolidação</v>
+            <v>Discussão pública</v>
           </cell>
           <cell r="K9" t="str">
             <v>Em andamento</v>
@@ -2113,7 +2555,7 @@
             <v>DOC, Jornal de grande circulação, Gestão Urbana, assessoria comunicação SMUL, email mailing colegiados, Prefeitura Regional</v>
           </cell>
           <cell r="CO9" t="str">
-            <v>Divulgada</v>
+            <v>Realizada</v>
           </cell>
           <cell r="CP9">
             <v>43242</v>
@@ -2128,7 +2570,7 @@
             <v>NC</v>
           </cell>
           <cell r="CT9" t="str">
-            <v>Reuniões bilaterais</v>
+            <v>Reuniões bilaterais com segmentos da sociedade civil</v>
           </cell>
           <cell r="CU9" t="str">
             <v>-</v>
@@ -3077,7 +3519,7 @@
             <v>Finalizado</v>
           </cell>
           <cell r="CY11" t="str">
-            <v>Não necessário</v>
+            <v>Diretrizes parcelamento e parâmetros urbanísticos</v>
           </cell>
           <cell r="CZ11" t="str">
             <v>Decreto</v>
@@ -3267,7 +3709,7 @@
             <v>Em tratativa na CMSP</v>
           </cell>
           <cell r="K12" t="str">
-            <v>Tramitação jurídica</v>
+            <v>Encaminhamento jurídico</v>
           </cell>
           <cell r="L12" t="str">
             <v>Ofício</v>
@@ -3408,7 +3850,7 @@
             <v>NA</v>
           </cell>
           <cell r="BF12">
-            <v>42919</v>
+            <v>42920</v>
           </cell>
           <cell r="BG12" t="str">
             <v>DDE-SPURB</v>
@@ -3444,7 +3886,7 @@
             <v>43139</v>
           </cell>
           <cell r="BR12">
-            <v>43139</v>
+            <v>43140</v>
           </cell>
           <cell r="BS12" t="str">
             <v>NA</v>
@@ -4232,8 +4674,8 @@
           <cell r="V14">
             <v>43265</v>
           </cell>
-          <cell r="W14" t="str">
-            <v>14/06/208</v>
+          <cell r="W14">
+            <v>43265</v>
           </cell>
           <cell r="X14">
             <v>43266</v>
@@ -4938,10 +5380,10 @@
             <v>Finalizado</v>
           </cell>
           <cell r="CY15" t="str">
-            <v>NA</v>
+            <v>Parâmetros para ZOE</v>
           </cell>
           <cell r="CZ15" t="str">
-            <v>Decreto (SPURB/DDE)</v>
+            <v>Decreto</v>
           </cell>
           <cell r="DA15" t="str">
             <v>NA</v>
@@ -4964,8 +5406,8 @@
           <cell r="DG15" t="str">
             <v>Parecer jurídico SPURBANISMO</v>
           </cell>
-          <cell r="DH15" t="str">
-            <v>11/05/2018 (TID:8328624)</v>
+          <cell r="DH15">
+            <v>43231</v>
           </cell>
           <cell r="DI15" t="str">
             <v>José Apparecido Jr.</v>
@@ -4977,7 +5419,7 @@
             <v>43231</v>
           </cell>
           <cell r="DL15" t="str">
-            <v xml:space="preserve">ATL (TID: 8393710) </v>
+            <v xml:space="preserve">ATL (TID: 8393710)  </v>
           </cell>
           <cell r="DM15" t="str">
             <v>Oficio AJ e Gabinete SMUL</v>
@@ -8367,7 +8809,7 @@
             <v>Em tratativa na CMSP</v>
           </cell>
           <cell r="K23" t="str">
-            <v>Tramitação jurídica</v>
+            <v>Encaminhamento jurídico</v>
           </cell>
           <cell r="L23" t="str">
             <v>NA</v>
@@ -8791,7 +9233,7 @@
             <v>PIU</v>
           </cell>
           <cell r="F24" t="str">
-            <v>PMSP - SMDP/SPP</v>
+            <v>PMSP - SMDP/SPP e SMT</v>
           </cell>
           <cell r="G24" t="str">
             <v>Decretos</v>
@@ -8818,7 +9260,7 @@
             <v>2017</v>
           </cell>
           <cell r="O24">
-            <v>42795</v>
+            <v>42767</v>
           </cell>
           <cell r="P24" t="str">
             <v>NA</v>
@@ -9160,10 +9602,9 @@
             <v>PMD</v>
           </cell>
           <cell r="DZ24" t="str">
-            <v xml:space="preserve">Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
-O Terminal Capelinha tem frentes para a Estrada de Itapecerica da Serra e a Av. Carlos Caldeira Filho, que ladeia o Córrego Morro do S. Além dessa avenida, implantado na encosta oeste do vale que define o córrego, há o Parque Munhoz, bairro consolidado conformado por condomínios de casas ou de apartamentos, sem áreas passíveis de transformação significativas. Apesar de mais de 57 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. 
-A transformação do perímetro do Terminal Campo Limpo deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. 
-Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 12 milhões, frente às receitas de pouco mais de R$ 600 mil. </v>
+            <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, potencializar atividades comerciais na área, acrescentar novos espaços e equipamentos públicos, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
+O Terminal Capelinha tem frentes para a Estrada de Itapecerica da Serra e situa-se em um bairro consolidado conformado por condomínios de casas ou de apartamentos, sem áreas passíveis de transformação significativas. Apesar de mais de 57 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. 
+Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 12 milhões, frente às receitas de pouco mais de R$ 600 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 83 milhões.</v>
           </cell>
           <cell r="EA24" t="str">
             <v>Receita: R$600mil
@@ -9256,7 +9697,7 @@
             <v>PIU</v>
           </cell>
           <cell r="F25" t="str">
-            <v>PMSP - SMDP/SPP</v>
+            <v>PMSP - SMDP/SPP e SMT</v>
           </cell>
           <cell r="G25" t="str">
             <v>Decretos</v>
@@ -9283,7 +9724,7 @@
             <v>2017</v>
           </cell>
           <cell r="O25">
-            <v>42795</v>
+            <v>42767</v>
           </cell>
           <cell r="P25" t="str">
             <v>NA</v>
@@ -9625,10 +10066,9 @@
             <v>PMD</v>
           </cell>
           <cell r="DZ25" t="str">
-            <v xml:space="preserve">Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
-O Terminal Campo Limpo está situado na divisa de São Paulo com Taboão da Serra, de forma que o âmbito de raio 600 m abrange áreas do município vizinho. Apesar de mais de 58 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. 
-A transformação do perímetro do Terminal Campo Limpo deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. 
-Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 8 milhões, frente às receitas de pouco mais de R$ 300 mil. </v>
+            <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
+O Terminal Campo Limpo está situado na divisa de São Paulo com Taboão da Serra. Apesar de mais de 58 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. 
+Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 8 milhões, frente às receitas de pouco mais de R$ 300 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 135 milhões.</v>
           </cell>
           <cell r="EA25" t="str">
             <v>Receita: R$300mil
@@ -9721,7 +10161,7 @@
             <v>PIU</v>
           </cell>
           <cell r="F26" t="str">
-            <v>PMSP - SMDP/SPP</v>
+            <v>PMSP - SMDP/SPP e SMT</v>
           </cell>
           <cell r="G26" t="str">
             <v>Decretos</v>
@@ -9748,7 +10188,7 @@
             <v>2017</v>
           </cell>
           <cell r="O26">
-            <v>42795</v>
+            <v>42767</v>
           </cell>
           <cell r="P26" t="str">
             <v>NA</v>
@@ -10090,12 +10530,10 @@
             <v>PMD</v>
           </cell>
           <cell r="DZ26" t="str">
-            <v xml:space="preserve">Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
-O perímetro proposto para o terminal Princesa Isabel praticamente corresponde ao polígono resultante da aplicação do círculo de 600 m de raio previsto em lei, abrangendo uma área de 100 ha. Situado na região central do município, adjacente a diversos equipamentos e áreas emblemáticas, envolve desde ZEIS-3, equipamentos tais como a Sala São Paulo, a Estação Pinacoteca, o Espaço Cultural Porto Seguro e o Sesc Bom Retiro, proximidade as estações de metrô Santa Cecília e da CPTM – Luz, conjunto de imóveis protegidos por órgãos de preservação no perímetro dos Campos Elíseos, assim como intervenções habitacionais de grande porte sendo realizada pelo Governo do Estado para implantação do Programa Casa Paulista. 
-Apesar de mais de 7 mil passageiros embarcarem diariamente no Terminal, a região adjacente a esse equipamento pouco se beneficia do potencial econômico que esse fluxo de pessoas pode trazer. Assim como outras áreas do centro da cidade, o entorno de Terminal Princesa Isabel é identificado como uma área inóspita, com tendência de esvaziamento noturno, grande número de pessoas em situação de rua e praças que servem de locais para deposição irregular de resíduos, dentre outras questões.
-A transformação do perímetro do Terminal Princesa Isabel deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. 
-Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 6 milhões, frente às receitas de pouco mais de R$ 200 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 75 milhões.
-</v>
+            <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. 
+O perímetro proposto para o terminal Princesa Isabel está situado na região central do município, próximo a diversos equipamentos e áreas emblemáticas, envolve áreas de ZEIS-3, equipamentos tais como a Sala São Paulo, a Estação Pinacoteca, o Espaço Cultural Porto Seguro e o Sesc Bom Retiro, proximidade as estações de metrô Santa Cecília e da CPTM – Luz, conjunto de imóveis protegidos por órgãos de preservação no perímetro dos Campos Elíseos, assim como intervenções habitacionais de grande porte sendo realizada pelo Governo do Estado para implantação do Programa Casa Paulista. 
+Apesar de mais de 7 mil passageiros embarcarem diariamente no Terminal, a região adjacente a esse equipamento pouco se beneficia do potencial econômico que esse fluxo de pessoas pode trazer.
+Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 6 milhões, frente às receitas de pouco mais de R$ 200 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 75 milhões.</v>
           </cell>
           <cell r="EA26" t="str">
             <v>Receita: R$200mil
@@ -10172,7 +10610,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
@@ -10180,6 +10617,7 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10477,7 +10915,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K26" sqref="K26"/>
+      <selection pane="bottomRight" sqref="A1:EX20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
@@ -10499,6 +10937,7 @@
     <col min="108" max="118" width="10.140625" customWidth="1"/>
     <col min="122" max="122" width="21.42578125" customWidth="1"/>
     <col min="125" max="125" width="14.140625" customWidth="1"/>
+    <col min="130" max="130" width="5" customWidth="1"/>
     <col min="141" max="141" width="6" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="10.5703125" customWidth="1"/>
   </cols>
@@ -11790,7 +12229,7 @@
       </c>
       <c r="J3" t="str">
         <f>CLEAN(IF([1]BD!J$6="P",[1]BD!J9,""))</f>
-        <v>Consolidação</v>
+        <v>Discussão pública</v>
       </c>
       <c r="K3" t="str">
         <f>CLEAN(IF([1]BD!K$6="P",[1]BD!K9,""))</f>
@@ -12142,7 +12581,7 @@
       </c>
       <c r="CT3" t="str">
         <f>CLEAN(IF([1]BD!CT$6="P",[1]BD!CT9,""))</f>
-        <v>Reuniões bilaterais</v>
+        <v>Reuniões bilaterais com segmentos da sociedade civil</v>
       </c>
       <c r="CU3" t="str">
         <f>CLEAN(IF([1]BD!CU$6="P",[1]BD!CU9,""))</f>
@@ -13398,7 +13837,7 @@
       </c>
       <c r="CY5" t="str">
         <f>CLEAN(IF([1]BD!CY$6="P",[1]BD!CY11,""))</f>
-        <v>Não necessário</v>
+        <v>Diretrizes parcelamento e parâmetros urbanísticos</v>
       </c>
       <c r="CZ5" t="str">
         <f>CLEAN(IF([1]BD!CZ$6="P",[1]BD!CZ11,""))</f>
@@ -13648,7 +14087,7 @@
       </c>
       <c r="K6" t="str">
         <f>CLEAN(IF([1]BD!K$6="P",[1]BD!K12,""))</f>
-        <v>Tramitação jurídica</v>
+        <v>Encaminhamento jurídico</v>
       </c>
       <c r="L6" t="str">
         <f>CLEAN(IF([1]BD!L$6="P",[1]BD!L12,""))</f>
@@ -13836,7 +14275,7 @@
       </c>
       <c r="BF6" t="str">
         <f>CLEAN(IF([1]BD!BF$6="P",[1]BD!BF12,""))</f>
-        <v>42919</v>
+        <v>42920</v>
       </c>
       <c r="BG6" t="str">
         <f>CLEAN(IF([1]BD!BG$6="P",[1]BD!BG12,""))</f>
@@ -13884,7 +14323,7 @@
       </c>
       <c r="BR6" t="str">
         <f>CLEAN(IF([1]BD!BR$6="P",[1]BD!BR12,""))</f>
-        <v>43139</v>
+        <v>43140</v>
       </c>
       <c r="BS6" t="str">
         <f>CLEAN(IF([1]BD!BS$6="P",[1]BD!BS12,""))</f>
@@ -14932,7 +15371,7 @@
       </c>
       <c r="W8" t="str">
         <f>CLEAN(IF([1]BD!W$6="P",[1]BD!W14,""))</f>
-        <v>14/06/208</v>
+        <v>43265</v>
       </c>
       <c r="X8" t="str">
         <f>CLEAN(IF([1]BD!X$6="P",[1]BD!X14,""))</f>
@@ -15870,11 +16309,11 @@
       </c>
       <c r="CY9" t="str">
         <f>CLEAN(IF([1]BD!CY$6="P",[1]BD!CY15,""))</f>
-        <v>NA</v>
+        <v>Parâmetros para ZOE</v>
       </c>
       <c r="CZ9" t="str">
         <f>CLEAN(IF([1]BD!CZ$6="P",[1]BD!CZ15,""))</f>
-        <v>Decreto (SPURB/DDE)</v>
+        <v>Decreto</v>
       </c>
       <c r="DA9" t="str">
         <f>CLEAN(IF([1]BD!DA$6="P",[1]BD!DA15,""))</f>
@@ -15906,7 +16345,7 @@
       </c>
       <c r="DH9" t="str">
         <f>CLEAN(IF([1]BD!DH$6="P",[1]BD!DH15,""))</f>
-        <v>11/05/2018 (TID:8328624)</v>
+        <v>43231</v>
       </c>
       <c r="DI9" t="str">
         <f>CLEAN(IF([1]BD!DI$6="P",[1]BD!DI15,""))</f>
@@ -18592,7 +19031,7 @@
       </c>
       <c r="K14" t="str">
         <f>CLEAN(IF([1]BD!K$6="P",[1]BD!K23,""))</f>
-        <v>Tramitação jurídica</v>
+        <v>Encaminhamento jurídico</v>
       </c>
       <c r="L14" t="str">
         <f>CLEAN(IF([1]BD!L$6="P",[1]BD!L23,""))</f>
@@ -19190,7 +19629,7 @@
       </c>
       <c r="F15" t="str">
         <f>CLEAN(IF([1]BD!F$6="P",[1]BD!F24,""))</f>
-        <v>PMSP - SMDP/SPP</v>
+        <v>PMSP - SMDP/SPP e SMT</v>
       </c>
       <c r="G15" t="str">
         <f>CLEAN(IF([1]BD!G$6="P",[1]BD!G24,""))</f>
@@ -19226,7 +19665,7 @@
       </c>
       <c r="O15" t="str">
         <f>CLEAN(IF([1]BD!O$6="P",[1]BD!O24,""))</f>
-        <v>42795</v>
+        <v>42767</v>
       </c>
       <c r="P15" t="str">
         <f>CLEAN(IF([1]BD!P$6="P",[1]BD!P24,""))</f>
@@ -19686,7 +20125,7 @@
       </c>
       <c r="DZ15" t="str">
         <f>CLEAN(IF([1]BD!DZ$6="P",[1]BD!DZ24,""))</f>
-        <v xml:space="preserve">Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. O Terminal Capelinha tem frentes para a Estrada de Itapecerica da Serra e a Av. Carlos Caldeira Filho, que ladeia o Córrego Morro do S. Além dessa avenida, implantado na encosta oeste do vale que define o córrego, há o Parque Munhoz, bairro consolidado conformado por condomínios de casas ou de apartamentos, sem áreas passíveis de transformação significativas. Apesar de mais de 57 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. A transformação do perímetro do Terminal Campo Limpo deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 12 milhões, frente às receitas de pouco mais de R$ 600 mil. </v>
+        <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, potencializar atividades comerciais na área, acrescentar novos espaços e equipamentos públicos, assim como apresentar modelo de financiamento e gestão do PIU em questão. O Terminal Capelinha tem frentes para a Estrada de Itapecerica da Serra e situa-se em um bairro consolidado conformado por condomínios de casas ou de apartamentos, sem áreas passíveis de transformação significativas. Apesar de mais de 57 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 12 milhões, frente às receitas de pouco mais de R$ 600 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 83 milhões.</v>
       </c>
       <c r="EA15" t="str">
         <f>CLEAN(IF([1]BD!EA$6="P",[1]BD!EA24,""))</f>
@@ -19808,7 +20247,7 @@
       </c>
       <c r="F16" t="str">
         <f>CLEAN(IF([1]BD!F$6="P",[1]BD!F25,""))</f>
-        <v>PMSP - SMDP/SPP</v>
+        <v>PMSP - SMDP/SPP e SMT</v>
       </c>
       <c r="G16" t="str">
         <f>CLEAN(IF([1]BD!G$6="P",[1]BD!G25,""))</f>
@@ -19844,7 +20283,7 @@
       </c>
       <c r="O16" t="str">
         <f>CLEAN(IF([1]BD!O$6="P",[1]BD!O25,""))</f>
-        <v>42795</v>
+        <v>42767</v>
       </c>
       <c r="P16" t="str">
         <f>CLEAN(IF([1]BD!P$6="P",[1]BD!P25,""))</f>
@@ -20304,7 +20743,7 @@
       </c>
       <c r="DZ16" t="str">
         <f>CLEAN(IF([1]BD!DZ$6="P",[1]BD!DZ25,""))</f>
-        <v xml:space="preserve">Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. O Terminal Campo Limpo está situado na divisa de São Paulo com Taboão da Serra, de forma que o âmbito de raio 600 m abrange áreas do município vizinho. Apesar de mais de 58 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. A transformação do perímetro do Terminal Campo Limpo deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 8 milhões, frente às receitas de pouco mais de R$ 300 mil. </v>
+        <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. O Terminal Campo Limpo está situado na divisa de São Paulo com Taboão da Serra. Apesar de mais de 58 mil passageiros embarcarem diariamente no Terminal, a região pouco se beneficia do potencial que esse fluxo de pessoas pode trazer. De acordo com a SP Trans, há inúmeros problemas de infraestrutura no Terminal Campo Limpo, envolvendo desde sua edificação, mobiliário, acessos, até seus sistemas de comunicação e de tecnologia de informação. Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 8 milhões, frente às receitas de pouco mais de R$ 300 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 135 milhões.</v>
       </c>
       <c r="EA16" t="str">
         <f>CLEAN(IF([1]BD!EA$6="P",[1]BD!EA25,""))</f>
@@ -22280,7 +22719,7 @@
       </c>
       <c r="F20" t="str">
         <f>CLEAN(IF([1]BD!F$6="P",[1]BD!F26,""))</f>
-        <v>PMSP - SMDP/SPP</v>
+        <v>PMSP - SMDP/SPP e SMT</v>
       </c>
       <c r="G20" t="str">
         <f>CLEAN(IF([1]BD!G$6="P",[1]BD!G26,""))</f>
@@ -22316,7 +22755,7 @@
       </c>
       <c r="O20" t="str">
         <f>CLEAN(IF([1]BD!O$6="P",[1]BD!O26,""))</f>
-        <v>42795</v>
+        <v>42767</v>
       </c>
       <c r="P20" t="str">
         <f>CLEAN(IF([1]BD!P$6="P",[1]BD!P26,""))</f>
@@ -22776,7 +23215,7 @@
       </c>
       <c r="DZ20" t="str">
         <f>CLEAN(IF([1]BD!DZ$6="P",[1]BD!DZ26,""))</f>
-        <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. O perímetro proposto para o terminal Princesa Isabel praticamente corresponde ao polígono resultante da aplicação do círculo de 600 m de raio previsto em lei, abrangendo uma área de 100 ha. Situado na região central do município, adjacente a diversos equipamentos e áreas emblemáticas, envolve desde ZEIS-3, equipamentos tais como a Sala São Paulo, a Estação Pinacoteca, o Espaço Cultural Porto Seguro e o Sesc Bom Retiro, proximidade as estações de metrô Santa Cecília e da CPTM – Luz, conjunto de imóveis protegidos por órgãos de preservação no perímetro dos Campos Elíseos, assim como intervenções habitacionais de grande porte sendo realizada pelo Governo do Estado para implantação do Programa Casa Paulista. Apesar de mais de 7 mil passageiros embarcarem diariamente no Terminal, a região adjacente a esse equipamento pouco se beneficia do potencial econômico que esse fluxo de pessoas pode trazer. Assim como outras áreas do centro da cidade, o entorno de Terminal Princesa Isabel é identificado como uma área inóspita, com tendência de esvaziamento noturno, grande número de pessoas em situação de rua e praças que servem de locais para deposição irregular de resíduos, dentre outras questões.A transformação do perímetro do Terminal Princesa Isabel deverá ocorrer através da recuperação dos espaços públicos de acesso preferencial ao Terminal e aos demais equipamentos existentes -  da requalificação de logradouros, da implementação de cruzamentos de pedestres, alargamento de calçadas e guias rebaixadas -  da arborização de vias -  da implantação de ciclovia/ciclofaixa -  dentre outras intervenções previstas. Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 6 milhões, frente às receitas de pouco mais de R$ 200 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 75 milhões.</v>
+        <v>Associados à Lei nº 16.211, que dispõe sobre a concessão para administração, manutenção, conservação, exploração comercial e requalificação de terminais de ônibus da cidade, e a redação dada pela Lei n. 16.703, de 04 de outubro de 2017, que estabelece a obrigatoriedade de realização de projetos de intervenção urbana para cada terminal de ônibus a ser desestatizado pelo Poder Público Municipal -  os PIUs dos Terminais (piloto), de proposição pública, buscam melhorias urbanísticas que garantam o pleno funcionamento do terminal, pretendem potencializar atividades comerciais na área, requalificar o uso residencial, acrescentar novos espaços e equipamentos públicos de qualidade, assim como apresentar modelo de financiamento e gestão do PIU em questão. O perímetro proposto para o terminal Princesa Isabel está situado na região central do município, próximo a diversos equipamentos e áreas emblemáticas, envolve áreas de ZEIS-3, equipamentos tais como a Sala São Paulo, a Estação Pinacoteca, o Espaço Cultural Porto Seguro e o Sesc Bom Retiro, proximidade as estações de metrô Santa Cecília e da CPTM – Luz, conjunto de imóveis protegidos por órgãos de preservação no perímetro dos Campos Elíseos, assim como intervenções habitacionais de grande porte sendo realizada pelo Governo do Estado para implantação do Programa Casa Paulista. Apesar de mais de 7 mil passageiros embarcarem diariamente no Terminal, a região adjacente a esse equipamento pouco se beneficia do potencial econômico que esse fluxo de pessoas pode trazer.Além da requalificação do Terminal e de seu perímetro de abrangência, O PIU pretende também realizar o equacionamento das condições de custeio do equipamento, que, anualmente, ultrapassa os R$ 6 milhões, frente às receitas de pouco mais de R$ 200 mil. Os investimentos previstos pelo PIU para a requalificação do perímetro de abrangência do Terminal Princesa Isabel são estimados em R$ 75 milhões.</v>
       </c>
       <c r="EA20" t="str">
         <f>CLEAN(IF([1]BD!EA$6="P",[1]BD!EA26,""))</f>
@@ -22880,146 +23319,285 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="83" priority="56" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="82" priority="55" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="81" priority="54" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="80" priority="53" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="79" priority="52" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="78" priority="51" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="77" priority="50" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="76" priority="49" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="75" priority="48" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="74" priority="47" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="73" priority="46" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="71" priority="44" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="70" priority="43" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="69" priority="42" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="68" priority="41" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="66" priority="39" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="65" priority="38" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="64" priority="37" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="61" priority="34" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="60" priority="33" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="59" priority="32" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="58" priority="31" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="53" priority="27" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="51" priority="26" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="49" priority="25" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="45" priority="23" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="43" priority="22" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="39" priority="20" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="33" priority="17" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="31" priority="16" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
+    <cfRule type="containsText" dxfId="27" priority="14" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
+    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:C20">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:C20">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20 C18 C20">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20 C18 C20">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finaliza primeira versao para publicar - com pagina completa piu setor central
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -69,7 +69,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="112">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1078,6 +1078,342 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -6512,6 +6848,9 @@
           </cell>
           <cell r="N18">
             <v>2017</v>
+          </cell>
+          <cell r="O18">
+            <v>43080</v>
           </cell>
           <cell r="P18" t="str">
             <v>NA</v>
@@ -17811,7 +18150,7 @@
       </c>
       <c r="O12" t="str">
         <f>CLEAN(IF([1]BD!O$6="P",[1]BD!O18,""))</f>
-        <v/>
+        <v>43080</v>
       </c>
       <c r="P12" t="str">
         <f>CLEAN(IF([1]BD!P$6="P",[1]BD!P18,""))</f>
@@ -23318,6 +23657,146 @@
       <c r="DU21" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="111" priority="84" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C17:C18 B17">
+    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="109" priority="82" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="108" priority="81" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="107" priority="80" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="106" priority="79" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="105" priority="78" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:C20">
+    <cfRule type="containsText" dxfId="104" priority="77" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="103" priority="76" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20 C18">
+    <cfRule type="containsText" dxfId="102" priority="75" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="101" priority="74" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="100" priority="73" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="99" priority="72" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="98" priority="71" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
+    <cfRule type="containsText" dxfId="97" priority="70" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B20 C17:C18 C20">
+    <cfRule type="containsText" dxfId="96" priority="69" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="95" priority="68" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="94" priority="67" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="93" priority="66" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="92" priority="65" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:C20">
+    <cfRule type="containsText" dxfId="91" priority="64" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:C20">
+    <cfRule type="containsText" dxfId="90" priority="63" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20 C18 C20">
+    <cfRule type="containsText" dxfId="89" priority="62" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B20 C18 C20">
+    <cfRule type="containsText" dxfId="88" priority="61" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="87" priority="60" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="86" priority="59" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="85" priority="58" operator="containsText" text="PIU">
+      <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="84" priority="57" operator="containsText" text="Projeto">
+      <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
     <cfRule type="containsText" dxfId="83" priority="56" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>

</xml_diff>

<commit_message>
Altera acj - responsavel (elaboracao)
</commit_message>
<xml_diff>
--- a/data_src/monitoramento.xlsx
+++ b/data_src/monitoramento.xlsx
@@ -69,7 +69,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="84">
     <dxf>
       <font>
         <condense val="0"/>
@@ -79,6 +79,18 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -110,11 +122,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -122,11 +134,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -158,11 +170,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -170,11 +182,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -206,11 +218,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -218,11 +230,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -254,11 +266,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -266,11 +278,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -302,11 +314,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -314,11 +326,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -350,30 +362,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -398,335 +386,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1434,11 +1098,6 @@
       <sheetName val="Personal"/>
       <sheetName val="História"/>
     </sheetNames>
-    <definedNames>
-      <definedName name="Menu_inicial"/>
-      <definedName name="SalvarBaseExterno"/>
-      <definedName name="writeToCSVfile"/>
-    </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
@@ -4190,9 +3849,6 @@
           </cell>
           <cell r="BG12" t="str">
             <v>DDE-SPURB</v>
-          </cell>
-          <cell r="BH12" t="str">
-            <v>Pedido de Prorrogação de Prazo (Conselho Gestor de SMUL)</v>
           </cell>
           <cell r="BI12" t="str">
             <v>Finalizada</v>
@@ -11251,10 +10907,10 @@
   <dimension ref="A1:FA21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:EX20"/>
+      <selection pane="bottomRight" activeCell="BH10" sqref="BH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15"/>
@@ -11272,6 +10928,7 @@
     <col min="24" max="24" width="11" customWidth="1"/>
     <col min="35" max="37" width="11.7109375" customWidth="1"/>
     <col min="58" max="58" width="14.7109375" customWidth="1"/>
+    <col min="60" max="60" width="38.42578125" customWidth="1"/>
     <col min="81" max="83" width="11.28515625" customWidth="1"/>
     <col min="108" max="118" width="10.140625" customWidth="1"/>
     <col min="122" max="122" width="21.42578125" customWidth="1"/>
@@ -14620,10 +14277,6 @@
         <f>CLEAN(IF([1]BD!BG$6="P",[1]BD!BG12,""))</f>
         <v>DDE-SPURB</v>
       </c>
-      <c r="BH6" t="str">
-        <f>CLEAN(IF([1]BD!BH$6="P",[1]BD!BH12,""))</f>
-        <v>Pedido de Prorrogação de Prazo (Conselho Gestor de SMUL)</v>
-      </c>
       <c r="BI6" t="str">
         <f>CLEAN(IF([1]BD!BI$6="P",[1]BD!BI12,""))</f>
         <v/>
@@ -23658,422 +23311,422 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="111" priority="84" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="83" priority="84" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="109" priority="82" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="81" priority="82" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="108" priority="81" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="107" priority="80" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="106" priority="79" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="105" priority="78" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="104" priority="77" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="103" priority="76" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="102" priority="75" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="101" priority="74" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="100" priority="73" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="99" priority="72" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="98" priority="71" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="97" priority="70" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="96" priority="69" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="95" priority="68" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="94" priority="67" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="93" priority="66" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="92" priority="65" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="91" priority="64" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="90" priority="63" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="89" priority="62" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="88" priority="61" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="87" priority="60" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="86" priority="59" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="85" priority="58" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="84" priority="57" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="83" priority="56" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="82" priority="55" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="81" priority="54" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="80" priority="53" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="79" priority="52" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="78" priority="51" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="77" priority="50" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="76" priority="49" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="75" priority="48" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="74" priority="47" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="73" priority="46" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="71" priority="44" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="70" priority="43" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="69" priority="42" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="68" priority="41" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="66" priority="39" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="65" priority="38" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="64" priority="37" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="61" priority="34" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="60" priority="33" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="59" priority="32" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="58" priority="31" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C17:C18 B17">
-    <cfRule type="containsText" dxfId="53" priority="27" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="51" priority="26" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="49" priority="25" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="45" priority="23" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="43" priority="22" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C20">
-    <cfRule type="containsText" dxfId="41" priority="21" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="39" priority="20" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20 C18">
-    <cfRule type="containsText" dxfId="37" priority="19" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="33" priority="17" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="31" priority="16" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="27" priority="14" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B20 C17:C18 C20">
-    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:C20">
-    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B20 C18 C20">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PIU">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="PIU">
       <formula>NOT(ISERROR(SEARCH("PIU",C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Projeto">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Projeto">
       <formula>NOT(ISERROR(SEARCH("Projeto",C20)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>